<commit_message>
50 klanten toegevoegd + omgezet naar csv-bestand
</commit_message>
<xml_diff>
--- a/RentACar/klanten.xlsx
+++ b/RentACar/klanten.xlsx
@@ -8,52 +8,39 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minne\RentACar\RentACar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0405CBC-911B-4305-80EB-BB5E4B1471E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF06FBA-A802-4F52-A407-020EE13E4A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="345" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Klanten" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="305">
   <si>
     <t>klantnummer</t>
   </si>
   <si>
-    <t>voornaam</t>
-  </si>
-  <si>
-    <t>naam</t>
-  </si>
-  <si>
-    <t>straat</t>
-  </si>
-  <si>
-    <t>straatnummer</t>
-  </si>
-  <si>
-    <t>busnummer</t>
-  </si>
-  <si>
-    <t>plaats</t>
-  </si>
-  <si>
-    <t>postcode</t>
-  </si>
-  <si>
-    <t>btw-nummer</t>
-  </si>
-  <si>
     <t>A-387-002</t>
   </si>
   <si>
@@ -205,16 +192,781 @@
   </si>
   <si>
     <t>Rijkevorsel</t>
+  </si>
+  <si>
+    <t>A-387-012</t>
+  </si>
+  <si>
+    <t>A-387-013</t>
+  </si>
+  <si>
+    <t>A-387-014</t>
+  </si>
+  <si>
+    <t>A-387-015</t>
+  </si>
+  <si>
+    <t>A-387-016</t>
+  </si>
+  <si>
+    <t>A-387-017</t>
+  </si>
+  <si>
+    <t>A-387-018</t>
+  </si>
+  <si>
+    <t>A-387-019</t>
+  </si>
+  <si>
+    <t>A-387-020</t>
+  </si>
+  <si>
+    <t>A-387-021</t>
+  </si>
+  <si>
+    <t>A-387-022</t>
+  </si>
+  <si>
+    <t>A-387-023</t>
+  </si>
+  <si>
+    <t>A-387-024</t>
+  </si>
+  <si>
+    <t>A-387-025</t>
+  </si>
+  <si>
+    <t>A-387-026</t>
+  </si>
+  <si>
+    <t>A-387-027</t>
+  </si>
+  <si>
+    <t>A-387-028</t>
+  </si>
+  <si>
+    <t>A-387-029</t>
+  </si>
+  <si>
+    <t>A-387-030</t>
+  </si>
+  <si>
+    <t>A-387-031</t>
+  </si>
+  <si>
+    <t>A-387-032</t>
+  </si>
+  <si>
+    <t>A-387-033</t>
+  </si>
+  <si>
+    <t>A-387-034</t>
+  </si>
+  <si>
+    <t>A-387-035</t>
+  </si>
+  <si>
+    <t>A-387-036</t>
+  </si>
+  <si>
+    <t>A-387-037</t>
+  </si>
+  <si>
+    <t>A-387-038</t>
+  </si>
+  <si>
+    <t>A-387-039</t>
+  </si>
+  <si>
+    <t>A-387-040</t>
+  </si>
+  <si>
+    <t>A-387-041</t>
+  </si>
+  <si>
+    <t>A-387-042</t>
+  </si>
+  <si>
+    <t>A-387-043</t>
+  </si>
+  <si>
+    <t>A-387-044</t>
+  </si>
+  <si>
+    <t>A-387-045</t>
+  </si>
+  <si>
+    <t>A-387-046</t>
+  </si>
+  <si>
+    <t>A-387-047</t>
+  </si>
+  <si>
+    <t>A-387-048</t>
+  </si>
+  <si>
+    <t>A-387-049</t>
+  </si>
+  <si>
+    <t>A-387-050</t>
+  </si>
+  <si>
+    <t>A-387-051</t>
+  </si>
+  <si>
+    <t>A-387-052</t>
+  </si>
+  <si>
+    <t>A-387-053</t>
+  </si>
+  <si>
+    <t>A-387-054</t>
+  </si>
+  <si>
+    <t>A-387-055</t>
+  </si>
+  <si>
+    <t>A-387-056</t>
+  </si>
+  <si>
+    <t>A-387-057</t>
+  </si>
+  <si>
+    <t>A-387-058</t>
+  </si>
+  <si>
+    <t>A-387-059</t>
+  </si>
+  <si>
+    <t>A-387-060</t>
+  </si>
+  <si>
+    <t>A-387-061</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>De Jong</t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>Jansen</t>
+  </si>
+  <si>
+    <t>Mila</t>
+  </si>
+  <si>
+    <t>De Vries</t>
+  </si>
+  <si>
+    <t>Sophie</t>
+  </si>
+  <si>
+    <t>Van Den Berg</t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>Yara</t>
+  </si>
+  <si>
+    <t>Saar</t>
+  </si>
+  <si>
+    <t>Nora</t>
+  </si>
+  <si>
+    <t>Tess</t>
+  </si>
+  <si>
+    <t>Noor</t>
+  </si>
+  <si>
+    <t>Milou</t>
+  </si>
+  <si>
+    <t>Sara</t>
+  </si>
+  <si>
+    <t>Liv</t>
+  </si>
+  <si>
+    <t>Zoë</t>
+  </si>
+  <si>
+    <t>Evi</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Luna</t>
+  </si>
+  <si>
+    <t>Lotte</t>
+  </si>
+  <si>
+    <t>Nina</t>
+  </si>
+  <si>
+    <t>Eva</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Lauren</t>
+  </si>
+  <si>
+    <t>Maeve</t>
+  </si>
+  <si>
+    <t>Lina</t>
+  </si>
+  <si>
+    <t>Elin</t>
+  </si>
+  <si>
+    <t>Noah</t>
+  </si>
+  <si>
+    <t>Liam</t>
+  </si>
+  <si>
+    <t>Luca</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Mees</t>
+  </si>
+  <si>
+    <t>Finn</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Milan</t>
+  </si>
+  <si>
+    <t>Levi</t>
+  </si>
+  <si>
+    <t>Sem</t>
+  </si>
+  <si>
+    <t>Daan</t>
+  </si>
+  <si>
+    <t>Noud</t>
+  </si>
+  <si>
+    <t>Luuk</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Bram</t>
+  </si>
+  <si>
+    <t>Zayn</t>
+  </si>
+  <si>
+    <t>Masom</t>
+  </si>
+  <si>
+    <t>Benjamin</t>
+  </si>
+  <si>
+    <t>Boaz</t>
+  </si>
+  <si>
+    <t>Siem</t>
+  </si>
+  <si>
+    <t>Guus</t>
+  </si>
+  <si>
+    <t>Morris</t>
+  </si>
+  <si>
+    <t>Olivier</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Van Dijk</t>
+  </si>
+  <si>
+    <t>Bakker</t>
+  </si>
+  <si>
+    <t>Janssen</t>
+  </si>
+  <si>
+    <t>Visser</t>
+  </si>
+  <si>
+    <t>Smit</t>
+  </si>
+  <si>
+    <t>Meijer</t>
+  </si>
+  <si>
+    <t>De Boer</t>
+  </si>
+  <si>
+    <t>Mulder</t>
+  </si>
+  <si>
+    <t>De Groot</t>
+  </si>
+  <si>
+    <t>Vos</t>
+  </si>
+  <si>
+    <t>Peters</t>
+  </si>
+  <si>
+    <t>Hendriks</t>
+  </si>
+  <si>
+    <t>Van Leeuwen</t>
+  </si>
+  <si>
+    <t>Dekker</t>
+  </si>
+  <si>
+    <t>De Wit</t>
+  </si>
+  <si>
+    <t>Brouwer</t>
+  </si>
+  <si>
+    <t>Dijkstra</t>
+  </si>
+  <si>
+    <t>Smits</t>
+  </si>
+  <si>
+    <t>De Graaf</t>
+  </si>
+  <si>
+    <t>Van Der Meer</t>
+  </si>
+  <si>
+    <t>Van Der Linden</t>
+  </si>
+  <si>
+    <t>De Cock</t>
+  </si>
+  <si>
+    <t>De Haan</t>
+  </si>
+  <si>
+    <t>Vermeulen</t>
+  </si>
+  <si>
+    <t>Van Den Heuvel</t>
+  </si>
+  <si>
+    <t>Van Der Steen</t>
+  </si>
+  <si>
+    <t>De Bruin</t>
+  </si>
+  <si>
+    <t>Schouten</t>
+  </si>
+  <si>
+    <t>Van Beek</t>
+  </si>
+  <si>
+    <t>Van Vliet</t>
+  </si>
+  <si>
+    <t>Scholliers</t>
+  </si>
+  <si>
+    <t>De Mol</t>
+  </si>
+  <si>
+    <t>De Kinder</t>
+  </si>
+  <si>
+    <t>Van Den Driesche</t>
+  </si>
+  <si>
+    <t>Maas</t>
+  </si>
+  <si>
+    <t>Verheyden</t>
+  </si>
+  <si>
+    <t>De Blom</t>
+  </si>
+  <si>
+    <t>Van Veen</t>
+  </si>
+  <si>
+    <t>Specter</t>
+  </si>
+  <si>
+    <t>De Ruiter</t>
+  </si>
+  <si>
+    <t>De Vos</t>
+  </si>
+  <si>
+    <t>Bosch</t>
+  </si>
+  <si>
+    <t>Timmermans</t>
+  </si>
+  <si>
+    <t>Van Doorn</t>
+  </si>
+  <si>
+    <t>Hooivelden</t>
+  </si>
+  <si>
+    <t>Kumtich</t>
+  </si>
+  <si>
+    <t>Kasterleesteenweg</t>
+  </si>
+  <si>
+    <t>Vechmaal</t>
+  </si>
+  <si>
+    <t>Ringlaan</t>
+  </si>
+  <si>
+    <t>Drieslinter</t>
+  </si>
+  <si>
+    <t>Prinsenstraat</t>
+  </si>
+  <si>
+    <t>Sprimont</t>
+  </si>
+  <si>
+    <t>Kapelaniestraat</t>
+  </si>
+  <si>
+    <t>Lichtervelde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strepestraat </t>
+  </si>
+  <si>
+    <t>Lambermont</t>
+  </si>
+  <si>
+    <t>Donk</t>
+  </si>
+  <si>
+    <t>Mandemakersstraat</t>
+  </si>
+  <si>
+    <t>Westrozebeek</t>
+  </si>
+  <si>
+    <t>Schoolstraat</t>
+  </si>
+  <si>
+    <t>Walcourt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Putstraat </t>
+  </si>
+  <si>
+    <t>Sint-Truiden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lange Elzenstraat </t>
+  </si>
+  <si>
+    <t>Bredene</t>
+  </si>
+  <si>
+    <t>Donceel</t>
+  </si>
+  <si>
+    <t>Lodewijk De Raetlaan</t>
+  </si>
+  <si>
+    <t>Ciply</t>
+  </si>
+  <si>
+    <t>Booischotseweg</t>
+  </si>
+  <si>
+    <t>Jauche</t>
+  </si>
+  <si>
+    <t>Rue De Fontigny</t>
+  </si>
+  <si>
+    <t>Rixensart</t>
+  </si>
+  <si>
+    <t>Rue Du Manoir</t>
+  </si>
+  <si>
+    <t>Agimont</t>
+  </si>
+  <si>
+    <t>Alsembergsesteenweg</t>
+  </si>
+  <si>
+    <t>Nieuwkerke</t>
+  </si>
+  <si>
+    <t>Westdorp</t>
+  </si>
+  <si>
+    <t>Tochogne</t>
+  </si>
+  <si>
+    <t>Rue De Virton</t>
+  </si>
+  <si>
+    <t>Ethe</t>
+  </si>
+  <si>
+    <t>Touslagerstraat</t>
+  </si>
+  <si>
+    <t>Zele</t>
+  </si>
+  <si>
+    <t>Rue Basse</t>
+  </si>
+  <si>
+    <t>Pittem</t>
+  </si>
+  <si>
+    <t>Stationsstraat</t>
+  </si>
+  <si>
+    <t>Incourt</t>
+  </si>
+  <si>
+    <t>Schietboompleinstraat</t>
+  </si>
+  <si>
+    <t>Ledegem</t>
+  </si>
+  <si>
+    <t>Leuze</t>
+  </si>
+  <si>
+    <t>Lanmbrechtstraat</t>
+  </si>
+  <si>
+    <t>Wemmel</t>
+  </si>
+  <si>
+    <t>Passiewijk</t>
+  </si>
+  <si>
+    <t>Neupré</t>
+  </si>
+  <si>
+    <t>Molenstraat</t>
+  </si>
+  <si>
+    <t>Sombreffe</t>
+  </si>
+  <si>
+    <t>Tisselt</t>
+  </si>
+  <si>
+    <t>Lodorp</t>
+  </si>
+  <si>
+    <t>Macon</t>
+  </si>
+  <si>
+    <t>Witbakkerstraat</t>
+  </si>
+  <si>
+    <t>Sint-Eloois-Vijve</t>
+  </si>
+  <si>
+    <t>Ramselsesteenweg</t>
+  </si>
+  <si>
+    <t>Lieferinge</t>
+  </si>
+  <si>
+    <t>Populierenstraat</t>
+  </si>
+  <si>
+    <t>Aarsele</t>
+  </si>
+  <si>
+    <t>Industriestraat</t>
+  </si>
+  <si>
+    <t>Deinze</t>
+  </si>
+  <si>
+    <t>Place Léopold</t>
+  </si>
+  <si>
+    <t>Herne</t>
+  </si>
+  <si>
+    <t>Tillet</t>
+  </si>
+  <si>
+    <t>Kortrijksteenweg</t>
+  </si>
+  <si>
+    <t>Tielt</t>
+  </si>
+  <si>
+    <t>Grote Beemd</t>
+  </si>
+  <si>
+    <t>Schilde</t>
+  </si>
+  <si>
+    <t>Noordhoekstraat</t>
+  </si>
+  <si>
+    <t>Veurne</t>
+  </si>
+  <si>
+    <t>Apostelblokweg</t>
+  </si>
+  <si>
+    <t>Holsbeek</t>
+  </si>
+  <si>
+    <t>Terheidelaan</t>
+  </si>
+  <si>
+    <t>Rotselaar</t>
+  </si>
+  <si>
+    <t>Pompeloerestraat</t>
+  </si>
+  <si>
+    <t>Sint-katelijneWaver</t>
+  </si>
+  <si>
+    <t>Bikschotestraat</t>
+  </si>
+  <si>
+    <t>Ieper</t>
+  </si>
+  <si>
+    <t>Pontweg</t>
+  </si>
+  <si>
+    <t>Lokeren</t>
+  </si>
+  <si>
+    <t>Sportstraat</t>
+  </si>
+  <si>
+    <t>Gent</t>
+  </si>
+  <si>
+    <t>Grote Molstenstraat</t>
+  </si>
+  <si>
+    <t>Kempestraat</t>
+  </si>
+  <si>
+    <t>Tierstraat</t>
+  </si>
+  <si>
+    <t>Diepenbeek</t>
+  </si>
+  <si>
+    <t>Reintjesbeek</t>
+  </si>
+  <si>
+    <t>Brasschaat</t>
+  </si>
+  <si>
+    <t>Gemeenteplein</t>
+  </si>
+  <si>
+    <t>Belseledorp</t>
+  </si>
+  <si>
+    <t>Sint-Niklaas</t>
+  </si>
+  <si>
+    <t>BE0495.55.653</t>
+  </si>
+  <si>
+    <t>BE0483.341.960</t>
+  </si>
+  <si>
+    <t>BE0428.867.211</t>
+  </si>
+  <si>
+    <t>BE0465.842.425</t>
+  </si>
+  <si>
+    <t>BE0484.786.648</t>
+  </si>
+  <si>
+    <t>Voornaam</t>
+  </si>
+  <si>
+    <t>Naam</t>
+  </si>
+  <si>
+    <t>Straat</t>
+  </si>
+  <si>
+    <t>Nummer</t>
+  </si>
+  <si>
+    <t>BusNr</t>
+  </si>
+  <si>
+    <t>Plaats</t>
+  </si>
+  <si>
+    <t>Postcode</t>
+  </si>
+  <si>
+    <t>BTW-nummer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -255,10 +1007,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -539,17 +1292,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -561,50 +1314,50 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
+      <c r="B1" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E2" s="2">
         <v>5</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H2" s="2">
         <v>2000</v>
@@ -613,23 +1366,23 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2">
         <v>78</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="H3" s="2">
         <v>9341</v>
@@ -638,23 +1391,23 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2">
         <v>321</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H4" s="2">
         <v>2300</v>
@@ -663,16 +1416,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2">
         <v>34</v>
@@ -681,7 +1434,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H5" s="2">
         <v>2543</v>
@@ -690,50 +1443,50 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E6" s="2">
         <v>57</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="H6" s="2">
         <v>9421</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2">
         <v>43</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H7" s="2">
         <v>7643</v>
@@ -742,23 +1495,23 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E8" s="2">
         <v>76</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H8" s="2">
         <v>3214</v>
@@ -767,16 +1520,16 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E9" s="2">
         <v>3</v>
@@ -785,7 +1538,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H9" s="2">
         <v>1000</v>
@@ -794,23 +1547,23 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E10" s="2">
         <v>77</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="H10" s="2">
         <v>9432</v>
@@ -819,30 +1572,1312 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E11" s="2">
         <v>31</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H11" s="2">
         <v>9021</v>
       </c>
       <c r="I11" s="2"/>
     </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E12" s="3">
+        <v>368</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="H12" s="3">
+        <v>3300</v>
+      </c>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E13" s="3">
+        <v>390</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="H13" s="3">
+        <v>3870</v>
+      </c>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="E14" s="3">
+        <v>371</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="H14" s="3">
+        <v>3350</v>
+      </c>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E15" s="3">
+        <v>376</v>
+      </c>
+      <c r="F15" s="2">
+        <v>2</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H15" s="3">
+        <v>9</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E16" s="3">
+        <v>134</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H16" s="3">
+        <v>8810</v>
+      </c>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E17" s="3">
+        <v>211</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="H17" s="3">
+        <v>4800</v>
+      </c>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="3">
+        <v>195</v>
+      </c>
+      <c r="F18" s="2">
+        <v>5</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="H18" s="3">
+        <v>3540</v>
+      </c>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E19" s="3">
+        <v>283</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="H19" s="3">
+        <v>8840</v>
+      </c>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E20" s="3">
+        <v>489</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="H20" s="3">
+        <v>5650</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E21" s="3">
+        <v>189</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="H21" s="3">
+        <v>3800</v>
+      </c>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E22" s="3">
+        <v>420</v>
+      </c>
+      <c r="F22" s="2">
+        <v>2</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="H22" s="3">
+        <v>8450</v>
+      </c>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="3">
+        <v>153</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="H23" s="3">
+        <v>4357</v>
+      </c>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="E24" s="3">
+        <v>149</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="H24" s="3">
+        <v>7024</v>
+      </c>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="E25" s="3">
+        <v>460</v>
+      </c>
+      <c r="F25" s="2">
+        <v>3</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="H25" s="3">
+        <v>1350</v>
+      </c>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="E26" s="3">
+        <v>11</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="H26" s="3">
+        <v>1330</v>
+      </c>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E27" s="3">
+        <v>455</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="H27" s="3">
+        <v>5544</v>
+      </c>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E28" s="3">
+        <v>426</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="H28" s="3">
+        <v>8950</v>
+      </c>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E29" s="3">
+        <v>455</v>
+      </c>
+      <c r="F29" s="2">
+        <v>2</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="H29" s="3">
+        <v>6941</v>
+      </c>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E30" s="3">
+        <v>44</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="H30" s="3">
+        <v>6760</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E31" s="3">
+        <v>241</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="H31" s="3">
+        <v>9240</v>
+      </c>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E32" s="3">
+        <v>142</v>
+      </c>
+      <c r="F32" s="2">
+        <v>3</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="H32" s="3">
+        <v>8740</v>
+      </c>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E33" s="3">
+        <v>211</v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="G33" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="H33" s="3">
+        <v>1315</v>
+      </c>
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="E34" s="3">
+        <v>52</v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="G34" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H34" s="3">
+        <v>8880</v>
+      </c>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E35" s="3">
+        <v>298</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="H35" s="3">
+        <v>5310</v>
+      </c>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E36" s="3">
+        <v>315</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="G36" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="H36" s="3">
+        <v>1780</v>
+      </c>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E37" s="3">
+        <v>23</v>
+      </c>
+      <c r="F37" s="2">
+        <v>1</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="H37" s="3">
+        <v>4120</v>
+      </c>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E38" s="3">
+        <v>420</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="G38" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="H38" s="3">
+        <v>5140</v>
+      </c>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E39" s="3">
+        <v>406</v>
+      </c>
+      <c r="F39" s="2"/>
+      <c r="G39" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="H39" s="3">
+        <v>2830</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="E40" s="3">
+        <v>17</v>
+      </c>
+      <c r="F40" s="2">
+        <v>4</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="H40" s="3">
+        <v>6591</v>
+      </c>
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="E41" s="3">
+        <v>415</v>
+      </c>
+      <c r="F41" s="2"/>
+      <c r="G41" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="H41" s="3">
+        <v>8793</v>
+      </c>
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E42" s="3">
+        <v>400</v>
+      </c>
+      <c r="F42" s="2"/>
+      <c r="G42" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H42" s="3">
+        <v>9400</v>
+      </c>
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E43" s="3">
+        <v>126</v>
+      </c>
+      <c r="F43" s="2"/>
+      <c r="G43" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="H43" s="3">
+        <v>8700</v>
+      </c>
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="E44" s="3">
+        <v>17</v>
+      </c>
+      <c r="F44" s="2"/>
+      <c r="G44" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="H44" s="3">
+        <v>9800</v>
+      </c>
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="E45" s="3">
+        <v>105</v>
+      </c>
+      <c r="F45" s="2"/>
+      <c r="G45" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="H45" s="3">
+        <v>1540</v>
+      </c>
+      <c r="I45" s="2"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E46" s="3">
+        <v>115</v>
+      </c>
+      <c r="F46" s="2"/>
+      <c r="G46" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="H46" s="3">
+        <v>6680</v>
+      </c>
+      <c r="I46" s="2"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E47" s="3">
+        <v>13</v>
+      </c>
+      <c r="F47" s="2"/>
+      <c r="G47" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="H47" s="3">
+        <v>8750</v>
+      </c>
+      <c r="I47" s="2"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E48" s="3">
+        <v>38</v>
+      </c>
+      <c r="F48" s="2"/>
+      <c r="G48" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="H48" s="3">
+        <v>2970</v>
+      </c>
+      <c r="I48" s="2"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="E49" s="3">
+        <v>1</v>
+      </c>
+      <c r="F49" s="2"/>
+      <c r="G49" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="H49" s="3">
+        <v>8630</v>
+      </c>
+      <c r="I49" s="2"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="E50" s="3">
+        <v>6</v>
+      </c>
+      <c r="F50" s="2"/>
+      <c r="G50" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="H50" s="3">
+        <v>3220</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="E51" s="3">
+        <v>61</v>
+      </c>
+      <c r="F51" s="2"/>
+      <c r="G51" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="H51" s="3">
+        <v>3110</v>
+      </c>
+      <c r="I51" s="2"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E52" s="3">
+        <v>36</v>
+      </c>
+      <c r="F52" s="2">
+        <v>1</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H52" s="3">
+        <v>2860</v>
+      </c>
+      <c r="I52" s="2"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="E53" s="3">
+        <v>44</v>
+      </c>
+      <c r="F53" s="2"/>
+      <c r="G53" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="H53" s="3">
+        <v>8920</v>
+      </c>
+      <c r="I53" s="2"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E54" s="3">
+        <v>50</v>
+      </c>
+      <c r="F54" s="2"/>
+      <c r="G54" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="H54" s="3">
+        <v>9160</v>
+      </c>
+      <c r="I54" s="2"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="E55" s="3">
+        <v>17</v>
+      </c>
+      <c r="F55" s="2"/>
+      <c r="G55" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="H55" s="3">
+        <v>9000</v>
+      </c>
+      <c r="I55" s="2"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="E56" s="2">
+        <v>14</v>
+      </c>
+      <c r="F56" s="2"/>
+      <c r="G56" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="H56" s="3">
+        <v>8710</v>
+      </c>
+      <c r="I56" s="2"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E57" s="2">
+        <v>16</v>
+      </c>
+      <c r="F57" s="2"/>
+      <c r="G57" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="H57" s="3">
+        <v>9800</v>
+      </c>
+      <c r="I57" s="2"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E58" s="2">
+        <v>41</v>
+      </c>
+      <c r="F58" s="2"/>
+      <c r="G58" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="H58" s="3">
+        <v>3590</v>
+      </c>
+      <c r="I58" s="2"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E59" s="2">
+        <v>25</v>
+      </c>
+      <c r="F59" s="2"/>
+      <c r="G59" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="H59" s="3">
+        <v>2930</v>
+      </c>
+      <c r="I59" s="2"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E60" s="2">
+        <v>10</v>
+      </c>
+      <c r="F60" s="2"/>
+      <c r="G60" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="H60" s="3">
+        <v>3806</v>
+      </c>
+      <c r="I60" s="2"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E61" s="2">
+        <v>165</v>
+      </c>
+      <c r="F61" s="2"/>
+      <c r="G61" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="H61" s="3">
+        <v>9111</v>
+      </c>
+      <c r="I61" s="2"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>